<commit_message>
La til første oppgavesett
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-V21.xlsx
+++ b/diverse/tidsplan-V21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakon/repositories/met4/diverse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB5C62D-C773-014C-ACC5-6F1806CA503B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EAFE1D-CAE3-42EB-A54C-577AA27D187D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="1905" windowWidth="19350" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Uke</t>
   </si>
@@ -84,7 +84,19 @@
     <t>21.01: Introduksjon til R på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
   </si>
   <si>
-    <t>28.01: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+    <t>28.01: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>02.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>04.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>09.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>11.02: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09). Se \@ref(seminar) for oppgaver.</t>
   </si>
 </sst>
 </file>
@@ -411,18 +423,18 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +448,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -450,7 +462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -464,23 +476,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -488,7 +512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -496,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -504,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -512,7 +536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -520,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -528,7 +552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>13</v>
       </c>
@@ -536,7 +560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -544,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
La til andre oppgaveseminar, nye datoer i tidsplanen
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-V21.xlsx
+++ b/diverse/tidsplan-V21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EAFE1D-CAE3-42EB-A54C-577AA27D187D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D953EB25-342E-4FD9-822B-C4C5DC21F717}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1905" windowWidth="19350" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="1950" windowWidth="24810" windowHeight="11115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Uke</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t>11.02: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>16.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>18.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>23.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>25.02: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>02.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>04.03: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09). Se \@ref(seminar) for oppgaver.</t>
   </si>
 </sst>
 </file>
@@ -423,7 +441,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,6 +529,12 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -519,6 +543,12 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -526,6 +556,12 @@
       </c>
       <c r="B8" t="s">
         <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Oppdatert tidsplan med oversiktsforelesninger
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-V21.xlsx
+++ b/diverse/tidsplan-V21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D953EB25-342E-4FD9-822B-C4C5DC21F717}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD723F0-FD35-4BD1-933F-EAE97533672C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="1950" windowWidth="24810" windowHeight="11115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22890" yWindow="420" windowWidth="15675" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Uke</t>
   </si>
@@ -115,6 +115,33 @@
   </si>
   <si>
     <t>04.03: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>09.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>11.03: **Oversiktsforelesning: Hypotesetesting** på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>16.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>18.03: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>23.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>25.03: **Oversiktsforelesning: Regresjon** på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>06.04: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>08.04: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>13.04: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
   </si>
 </sst>
 </file>
@@ -441,7 +468,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,6 +598,12 @@
       <c r="B9" t="s">
         <v>13</v>
       </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -579,6 +612,12 @@
       <c r="B10" t="s">
         <v>9</v>
       </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -587,6 +626,12 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -603,6 +648,12 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -610,6 +661,9 @@
       </c>
       <c r="B14" t="s">
         <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rettet feil dato for gjesteforelesning
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-V21.xlsx
+++ b/diverse/tidsplan-V21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD723F0-FD35-4BD1-933F-EAE97533672C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1F9740-D8CC-487B-AD11-538B265FF5A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22890" yWindow="420" windowWidth="15675" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Uke</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>13.04: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
+  </si>
+  <si>
+    <t>15.04: Gjesteforelesning med Ole-Petter Hansen, Tryg Forsikring  på [Zoom](https://nhh.zoom.us/j/63633653066?pwd=cTVNV0JvOXl4NnUrMHVKdkw2b0pCZz09).</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,6 +668,9 @@
       <c r="C14" t="s">
         <v>38</v>
       </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>